<commit_message>
changed db from mongoDB to PostgreSQL, added error handling
</commit_message>
<xml_diff>
--- a/Errors with coresponding codes.xlsx
+++ b/Errors with coresponding codes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Log analysis\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\log_analysis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20128B0A-6613-46C0-B6F9-0DE715B393DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E848EE-016D-4F3A-9E84-E653F8AB7793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Číslo chyby</t>
   </si>
@@ -84,6 +84,36 @@
   </si>
   <si>
     <t>RECORD_INVALID</t>
+  </si>
+  <si>
+    <t>VERSION_INVALID</t>
+  </si>
+  <si>
+    <t>V zadanom zázname neexistuje verzia</t>
+  </si>
+  <si>
+    <t>VERSION_UNAVAILABLE</t>
+  </si>
+  <si>
+    <t>Zadaná verzia nespĺňa kritéria pre SW ver. 2G ani 3G</t>
+  </si>
+  <si>
+    <t>NO_PROCESSED_RECORDS</t>
+  </si>
+  <si>
+    <t>Žiaden zo záznamov sa nepodarilo spracovať</t>
+  </si>
+  <si>
+    <t>Kontrola formátu záznamu príp. Jeho úprava</t>
+  </si>
+  <si>
+    <t>MISSING_SAFE_BITES</t>
+  </si>
+  <si>
+    <t>V zázname neboli nájdené safe bytes</t>
+  </si>
+  <si>
+    <t>Doplniť chýbajúce safe bytes</t>
   </si>
 </sst>
 </file>
@@ -139,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D6" totalsRowShown="0">
-  <autoFilter ref="A1:D6" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
+  <autoFilter ref="A1:D10" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9BB2DB52-04BA-41D4-AFFE-7C28DF31BD54}" name="Číslo chyby"/>
     <tableColumn id="2" xr3:uid="{2AE8D65E-8AE0-4280-B392-4D9AC6553123}" name="Názov"/>
@@ -448,16 +478,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566C1D1E-1707-43F6-B3F0-F6149F033DA6}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
@@ -519,6 +549,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -527,8 +560,61 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>104</v>
+      </c>
       <c r="B6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added paths to file object
</commit_message>
<xml_diff>
--- a/Errors with coresponding codes.xlsx
+++ b/Errors with coresponding codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\log_analysis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E848EE-016D-4F3A-9E84-E653F8AB7793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79F190-2D6E-4D24-9663-2D8135A8C250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Číslo chyby</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Doplniť chýbajúce safe bytes</t>
+  </si>
+  <si>
+    <t>SESSION_FAILED</t>
+  </si>
+  <si>
+    <t>Nebolo možné utvoriť reláciu medzi databázou a klientom</t>
+  </si>
+  <si>
+    <t>Skontrolovať prihlasovacie údaje</t>
+  </si>
+  <si>
+    <t>REFFERENCES_RETRIEVAL_FAILURE</t>
+  </si>
+  <si>
+    <t>Kontaktovať administrátora</t>
+  </si>
+  <si>
+    <t>Pri sťahovaní dát z jednej z tabuliek: Path,Actor,Board,HDV,Software nastala chyba</t>
   </si>
 </sst>
 </file>
@@ -169,8 +187,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9BB2DB52-04BA-41D4-AFFE-7C28DF31BD54}" name="Číslo chyby"/>
     <tableColumn id="2" xr3:uid="{2AE8D65E-8AE0-4280-B392-4D9AC6553123}" name="Názov"/>
@@ -478,17 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566C1D1E-1707-43F6-B3F0-F6149F033DA6}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -615,6 +633,34 @@
       </c>
       <c r="D10" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed extracting regex, to unify record formatting
</commit_message>
<xml_diff>
--- a/Errors with coresponding codes.xlsx
+++ b/Errors with coresponding codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\log_analysis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52804E1-93A4-4583-8650-C08BE88C9EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233776A0-D598-4753-BD83-7CC9BD3743DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Názov</t>
   </si>
@@ -77,9 +77,6 @@
     <t>RECORD_DUPLICATE</t>
   </si>
   <si>
-    <t>Záznam je potvrdením duplikátom už existujúceho záznamu</t>
-  </si>
-  <si>
     <t>RECORD_INVALID</t>
   </si>
   <si>
@@ -141,6 +138,24 @@
   </si>
   <si>
     <t>Požiadavka na ukončenie spracovávania, upload</t>
+  </si>
+  <si>
+    <t>Pre dopytovaný súbor nebolo možné nájsť enkódovanie. Testované sú formáty utf-8</t>
+  </si>
+  <si>
+    <t>Záznam je potvrdeným duplikátom už existujúceho záznamu</t>
+  </si>
+  <si>
+    <t>DECODING_FAILURE</t>
+  </si>
+  <si>
+    <t>UNSUPPORTED_LOG</t>
+  </si>
+  <si>
+    <t>Skontrolujte, že názov súboru obsahuje "KAM" alebo "PAP" a príponu .log</t>
+  </si>
+  <si>
+    <t>Zvolený súbor nie je podporovaný log (PAP, KAM resp. PAP a KAM)</t>
   </si>
 </sst>
 </file>
@@ -196,8 +211,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0">
-  <autoFilter ref="A1:D14" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0">
+  <autoFilter ref="A1:D16" xr:uid="{3C35F16D-D6C0-4895-998E-A963FDAD4C3B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9BB2DB52-04BA-41D4-AFFE-7C28DF31BD54}" name="Číslo hlásenia"/>
     <tableColumn id="2" xr3:uid="{2AE8D65E-8AE0-4280-B392-4D9AC6553123}" name="Názov"/>
@@ -505,23 +520,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566C1D1E-1707-43F6-B3F0-F6149F033DA6}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -533,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -547,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101</v>
       </c>
@@ -561,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
@@ -575,7 +590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>103</v>
       </c>
@@ -583,112 +598,137 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>105</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>106</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>107</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>108</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>109</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
       <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>111</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>200</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
+      <c r="B16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for windows-1250 encoded files and created more robust system for capturing exception
</commit_message>
<xml_diff>
--- a/Errors with coresponding codes.xlsx
+++ b/Errors with coresponding codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\log_analysis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEDFE11-EAB4-42C1-92D8-104A685795F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECF5CA2-1F1C-435E-94A2-9C2B10518A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Názov</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Požiadavka na ukončenie spracovávania, upload</t>
   </si>
   <si>
-    <t>Pre dopytovaný súbor nebolo možné nájsť enkódovanie. Testované sú formáty utf-8</t>
-  </si>
-  <si>
     <t>Záznam je potvrdeným duplikátom už existujúceho záznamu</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>UNSUPPORTED_LOG</t>
   </si>
   <si>
-    <t>Skontrolujte, že názov súboru obsahuje "KAM" alebo "PAP" a príponu .log</t>
-  </si>
-  <si>
     <t>Zvolený súbor nie je podporovaný log (PAP, KAM resp. PAP a KAM)</t>
   </si>
   <si>
@@ -165,6 +159,15 @@
   </si>
   <si>
     <t>Preklep, syntaktická chyba?</t>
+  </si>
+  <si>
+    <t>Manuálne otvoriť súbor a zmenit enkódovanie na jeden z podporovaných formátov</t>
+  </si>
+  <si>
+    <t>Skontrolujte, že názov súboru obsahuje "KAM" alebo "PAP" a príponu .log resp .txt</t>
+  </si>
+  <si>
+    <t>Pre dopytovaný súbor nebolo možné nájsť enkódovanie. Testované sú formáty UTF-16, UTF-8 a windows-1250</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +543,7 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,10 +715,13 @@
         <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -723,13 +729,13 @@
         <v>113</v>
       </c>
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,13 +743,13 @@
         <v>114</v>
       </c>
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Preparing ofr another paramaeter validation
</commit_message>
<xml_diff>
--- a/Errors with coresponding codes.xlsx
+++ b/Errors with coresponding codes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\log_analysis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECF5CA2-1F1C-435E-94A2-9C2B10518A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7B2B89-2385-4C87-945F-8D5960236BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{393BC539-5651-4F97-AB2A-439B31DC9896}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Názov</t>
   </si>
@@ -168,16 +169,218 @@
   </si>
   <si>
     <t>Pre dopytovaný súbor nebolo možné nájsť enkódovanie. Testované sú formáty UTF-16, UTF-8 a windows-1250</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\03\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\05\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\05\PC_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\06\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\09\MO_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\02\TN_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\03\PV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\09\OZP_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\10\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\11\EN_OZP_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\PH_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\VS_PAPlog nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\03\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\08\EN_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\11\MO_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\02\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\04\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\06\MM_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\06\PH_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\07\VA_lamw.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\02\AL_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\JD_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\VA_.LOG nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\AL_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\EN_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\MO_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\RD_AP.LOG.txt nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\11\AL_.LOG nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\01\kvB_amw.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\OZP28_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\10\PH_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\12\TU_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2018\04\TU_MAP_DAM3G_20180411_105836.log nie je log typu KAM ani PAP. FILE_SKIPPED       </t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\09\VL_AP_2019-09.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor c:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\12\VS_AP_2019-12.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Povodne</t>
+  </si>
+  <si>
+    <t>Opravene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\02\TN_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\03\PV_.log nie je log </t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\09\OZP_.log nie je log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\10\AV_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\11\EN_OZP_.log nie je </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\PH_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\03\AV_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\08\EN_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\11\MO_.log nie je log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\12\VA_.log nie je log </t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\02\IvB_.log nie je log</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\04\IvB_.log nie je log</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\09\VL_AP_2019-09.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\12\VS_AP_2019-12.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\03\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\05\AV_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\05\PC_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\06\IvB_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>Chyba 113: Súbor C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\09\MO_.log nie je log typu KAM ani PAP. FILE_SKIPPED</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\12\VS_AP_2019-12.log</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\03\AV_.log</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\05\AV_.log</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\05\PC_.log</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\06\IvB_.log</t>
+  </si>
+  <si>
+    <t>C:\Users\Simon\Desktop\log_analysis\data\operation logs\old\2012\09\MO_.log</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,8 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566C1D1E-1707-43F6-B3F0-F6149F033DA6}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,4 +973,730 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2673D21D-A342-4325-9CC5-CAFC26B2E448}">
+  <dimension ref="A1:Q39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="104" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="str">
+        <f>LEFT(RIGHT(A2,LEN(A2)-17),LEN(RIGHT(A2,LEN(A2)-17))-42)</f>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\03\AV_.log</v>
+      </c>
+      <c r="C2">
+        <f>+_xlfn.XMATCH(E2,B2:B39)</f>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="str">
+        <f>LEFT(RIGHT(D2,LEN(D2)-17),LEN(RIGHT(D2,LEN(D2)-17))-12)</f>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\02\TN_.log</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B39" si="0">LEFT(RIGHT(A3,LEN(A3)-17),LEN(RIGHT(A3,LEN(A3)-17))-42)</f>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\05\AV_.log</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C19" si="1">+_xlfn.XMATCH(E3,B3:B40)</f>
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E13" si="2">LEFT(RIGHT(D3,LEN(D3)-17),LEN(RIGHT(D3,LEN(D3)-17))-12)</f>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\03\PV_.log</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\05\PC_.log</v>
+      </c>
+      <c r="C4" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\09\OZP_.lo</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\06\IvB_.log</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\10\AV_.log</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2012\09\MO_.log</v>
+      </c>
+      <c r="C6" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\11\EN_OZP_</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\02\TN_.log</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\PH_.log</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\03\PV_.log</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\03\AV_.log</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\09\OZP_.log</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\08\EN_.log</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\10\AV_.log</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\11\MO_.log</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2013\11\EN_OZP_.log</v>
+      </c>
+      <c r="C11" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\12\VA_.log</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\PH_.log</v>
+      </c>
+      <c r="C12" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\02\IvB_.lo</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\02\VS_PAPlog</v>
+      </c>
+      <c r="C13" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>C:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\04\IvB_.lo</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\03\AV_.log</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\08\EN_.log</v>
+      </c>
+      <c r="C15" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2014\11\MO_.log</v>
+      </c>
+      <c r="C16" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\02\IvB_.log</v>
+      </c>
+      <c r="C17" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\04\IvB_.log</v>
+      </c>
+      <c r="C18" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\06\MM_.log</v>
+      </c>
+      <c r="C19" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\06\PH_.log</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2015\07\VA_lamw.log</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\02\AL_.log</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\IvB_.log</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\03\JD_.log</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\IvB_.log</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\04\VA_.LOG</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\AL_.log</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\EN_.log</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\MO_.log</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\05\RD_AP.LOG.txt</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2016\11\AL_.LOG</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\01\kvB_amw.log</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\IvB_.log</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\06\OZP28_.log</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\10\PH_.log</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2017\12\TU_.log</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2018\04\TU_MAP_DAM3G_20180411_105836.log nie je</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\09\VL_AP_2019-09.log</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>c:\Users\Simon\Desktop\log_analysis\data\operation logs\2019\12\VS_AP_2019-12.log</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>